<commit_message>
Changed report template format.
</commit_message>
<xml_diff>
--- a/templates/summary_template.xlsx
+++ b/templates/summary_template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\ISDP\3_Projects\1_City_Wide\Monitoring\Data_Management\400_Project_Work\R Tools\scattergraph_app_github\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE3D2E24-FED7-4107-A4FC-F514E5614880}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C66B7E39-0656-429A-A049-41A766D122F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{24220EFC-B0E4-4609-8325-DAA514CAF531}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{24220EFC-B0E4-4609-8325-DAA514CAF531}"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
   </sheets>
   <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="3" r:id="rId4"/>
+    <pivotCache cacheId="1" r:id="rId4"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -195,6 +195,1608 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-CA"/>
+              <a:t>Scattergraph</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="smoothMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>Observed</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="diamond"/>
+            <c:size val="2"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent6">
+                  <a:lumMod val="50000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent6">
+                    <a:lumMod val="50000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Data!$C$2:$C$29187</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="29186"/>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Data!$B$2:$B$29187</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="29186"/>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-075D-4139-91DF-AFB08A247B4D}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>Design Method</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Scattergraph_Data!$L$2:$L$1001</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="1000"/>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Scattergraph_Data!$C$2:$C$1001</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="1000"/>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-075D-4139-91DF-AFB08A247B4D}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:v>LC Method</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Scattergraph_Data!$M$2:$M$1001</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="1000"/>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Scattergraph_Data!$C$2:$C$1001</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="1000"/>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-075D-4139-91DF-AFB08A247B4D}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:v>SS Method</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Scattergraph_Data!$N$2:$N$1001</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="1000"/>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Scattergraph_Data!$C$2:$C$1001</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="1000"/>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-075D-4139-91DF-AFB08A247B4D}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="4"/>
+          <c:tx>
+            <c:v>Froude 0.7</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent5"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Scattergraph_Data!$Q$2:$Q$1001</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="1000"/>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Scattergraph_Data!$C$2:$C$1001</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="1000"/>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000005-075D-4139-91DF-AFB08A247B4D}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="5"/>
+          <c:order val="5"/>
+          <c:tx>
+            <c:v>Froude 1.0</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent6"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Scattergraph_Data!$R$2:$R$1001</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="1000"/>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Scattergraph_Data!$C$2:$C$1001</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="1000"/>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000006-075D-4139-91DF-AFB08A247B4D}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="6"/>
+          <c:order val="6"/>
+          <c:tx>
+            <c:v>Froude 1.5</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1">
+                  <a:lumMod val="60000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Scattergraph_Data!$S$2:$S$1001</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="1000"/>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Scattergraph_Data!$C$2:$C$1001</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="1000"/>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000007-075D-4139-91DF-AFB08A247B4D}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="7"/>
+          <c:order val="7"/>
+          <c:tx>
+            <c:v>2% iso Q</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2">
+                  <a:lumMod val="60000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Scattergraph_Data!$U$2:$U$1001</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="1000"/>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Scattergraph_Data!$C$2:$C$1001</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="1000"/>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000008-075D-4139-91DF-AFB08A247B4D}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="8"/>
+          <c:order val="8"/>
+          <c:tx>
+            <c:v>5% iso Q</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent3">
+                  <a:lumMod val="60000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Scattergraph_Data!$V$2:$V$1001</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="1000"/>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Scattergraph_Data!$C$2:$C$1001</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="1000"/>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000009-075D-4139-91DF-AFB08A247B4D}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="9"/>
+          <c:order val="9"/>
+          <c:tx>
+            <c:v>10% iso Q</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent4">
+                  <a:lumMod val="60000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Scattergraph_Data!$W$2:$W$1001</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="1000"/>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Scattergraph_Data!$C$2:$C$1001</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="1000"/>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{0000000A-075D-4139-91DF-AFB08A247B4D}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="10"/>
+          <c:order val="10"/>
+          <c:tx>
+            <c:v>15% iso Q</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent5">
+                  <a:lumMod val="60000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Scattergraph_Data!$X$2:$X$1001</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="1000"/>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Scattergraph_Data!$C$2:$C$1001</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="1000"/>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{0000000B-075D-4139-91DF-AFB08A247B4D}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="11"/>
+          <c:order val="11"/>
+          <c:tx>
+            <c:v>20% iso Q</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent6">
+                  <a:lumMod val="60000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Scattergraph_Data!$Y$2:$Y$1001</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="1000"/>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Scattergraph_Data!$C$2:$C$1001</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="1000"/>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{0000000C-075D-4139-91DF-AFB08A247B4D}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="12"/>
+          <c:order val="12"/>
+          <c:tx>
+            <c:v>25% iso Q</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1">
+                  <a:lumMod val="80000"/>
+                  <a:lumOff val="20000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Scattergraph_Data!$Z$2:$Z$1001</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="1000"/>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Scattergraph_Data!$C$2:$C$1001</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="1000"/>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{0000000D-075D-4139-91DF-AFB08A247B4D}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="1250743520"/>
+        <c:axId val="1250744000"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="1250743520"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="10"/>
+          <c:min val="0"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-CA"/>
+                  <a:t>Velocity</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-CA" baseline="0"/>
+                  <a:t> (m/s)</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-CA"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1250744000"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="1250744000"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-CA"/>
+                  <a:t>Depth</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-CA" baseline="0"/>
+                  <a:t> (mm)</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-CA"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1250743520"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>571500</xdr:colOff>
+      <xdr:row>58</xdr:row>
+      <xdr:rowOff>138113</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F6412E18-EE17-47CA-A23A-BF90D0F28846}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -437,7 +2039,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{D8E3E6BF-D706-44B1-B0D9-6AB6FF99F00D}" name="PivotTable1" cacheId="3" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{D8E3E6BF-D706-44B1-B0D9-6AB6FF99F00D}" name="PivotTable1" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="I9:O12" firstHeaderRow="0" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="7">
     <pivotField numFmtId="22" showAll="0">
@@ -975,8 +2577,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C524CA24-CD47-4AC9-914E-B2928D65A01F}">
   <dimension ref="A1:P60"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J14" sqref="J14"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="L37" sqref="L37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1582,6 +3184,7 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId2"/>
+  <drawing r:id="rId3"/>
 </worksheet>
 </file>
 
@@ -1589,7 +3192,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DCFEA426-6D11-4F6C-AD1E-EFD0536DFD16}">
   <dimension ref="A2:A6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
@@ -1625,7 +3228,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{50774F5E-D13F-476B-AB71-C4B92A1CC9F7}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>

</xml_diff>